<commit_message>
catch_yandex after first test
</commit_message>
<xml_diff>
--- a/Exel/data.xlsx
+++ b/Exel/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,11 +603,16 @@
           <t>courier_phone</t>
         </is>
       </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>img</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>420311</t>
+          <t>2b0ef515-52f1-4a81-a467-c9253eeb31ed</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -624,7 +629,7 @@
         <v>21</v>
       </c>
       <c r="E2" t="n">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c r="F2" t="n">
         <v>99</v>
@@ -641,11 +646,11 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1965</v>
+        <v>2000</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Pavel</t>
+          <t>Павел</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -663,7 +668,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>+79175706804</t>
+          <t>+79161052259</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -677,30 +682,30 @@
         </is>
       </c>
       <c r="R2" s="2" t="n">
-        <v>45162.85416666666</v>
+        <v>45177.41666666666</v>
       </c>
       <c r="S2" s="2" t="n">
-        <v>45162.89583333334</v>
+        <v>45177.45833333334</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>https://apitest.dostavista.ru/track/PG7IMW4AZY7GRU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>https://apitest.dostavista.ru/track/PGESEJRR92PERU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="n">
-        <v>45229</v>
+        <v>46386</v>
       </c>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Москва, Фестивальная улица, 22к7</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -714,17 +719,16 @@
         </is>
       </c>
       <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="n">
-        <v>45236</v>
-      </c>
+      <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>52398767</t>
+          <t>4e7f49dd-5066-4462-a6cd-0317f9e023dd</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -741,7 +745,7 @@
         <v>21</v>
       </c>
       <c r="E3" t="n">
-        <v>174</v>
+        <v>234</v>
       </c>
       <c r="F3" t="n">
         <v>99</v>
@@ -758,11 +762,11 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>1903</v>
+        <v>1963</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Pavel</t>
+          <t>Павел</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -790,41 +794,41 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>tomorrow</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="R3" s="2" t="n">
-        <v>45164.875</v>
+        <v>45183.4375</v>
       </c>
       <c r="S3" s="2" t="n">
-        <v>45164.91666666666</v>
+        <v>45183.47916666666</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PGHR7JXI7IPIRU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PGA21J4J95EYRU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="n">
-        <v>45589</v>
+        <v>46848</v>
       </c>
       <c r="Y3" t="n">
-        <v>45595</v>
+        <v>46854</v>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>canceled</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>waiting</t>
+          <t>end_collect</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -833,17 +837,16 @@
         </is>
       </c>
       <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="n">
-        <v>45596</v>
-      </c>
+      <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>52400702</t>
+          <t>54255388</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -860,7 +863,7 @@
         <v>21</v>
       </c>
       <c r="E4" t="n">
-        <v>223</v>
+        <v>273</v>
       </c>
       <c r="F4" t="n">
         <v>99</v>
@@ -877,7 +880,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>1952</v>
+        <v>2002</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -913,43 +916,37 @@
         </is>
       </c>
       <c r="R4" s="2" t="n">
-        <v>45163.875</v>
+        <v>45182.875</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>45163.91666666666</v>
+        <v>45182.91666666666</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PGHD9IZGH5DNRU</t>
+          <t>https://dostavista.ru/track/PGLTIG1PIJH2RU</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PG3LZ4LMFW3YRU</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>за 5 минут до доставки позвонить</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>к упаковке добавить записку</t>
-        </is>
-      </c>
+          <t>https://dostavista.ru/track/PGEDGX3532S7RU</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="n">
-        <v>45649</v>
-      </c>
-      <c r="Y4" t="inlineStr"/>
+        <v>46555</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>46563</v>
+      </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>finished</t>
+          <t>canceled</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>waiting</t>
+          <t>waiting_photo</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
@@ -959,26 +956,19 @@
       </c>
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="n">
-        <v>45655</v>
+        <v>46561</v>
       </c>
       <c r="AE4" t="n">
-        <v>45656</v>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+        <v>46562</v>
+      </c>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>52311577</t>
+          <t>9f5490f0-5ce4-458f-9901-d1c42f8180c0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -995,7 +985,7 @@
         <v>21</v>
       </c>
       <c r="E5" t="n">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F5" t="n">
         <v>99</v>
@@ -1012,7 +1002,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>1969</v>
+        <v>1963</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -1044,38 +1034,34 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Today</t>
+          <t>tomorrow</t>
         </is>
       </c>
       <c r="R5" s="2" t="n">
-        <v>45162.85416666666</v>
+        <v>45183.41666666666</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>45162.875</v>
+        <v>45183.45833333334</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PG2PJFAMK33RRU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PGCRSRGX1WMERU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>За 10 минут</t>
-        </is>
-      </c>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="n">
-        <v>45301</v>
+        <v>46758</v>
       </c>
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>finished</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
@@ -1089,27 +1075,16 @@
         </is>
       </c>
       <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="n">
-        <v>45308</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>45309</v>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>52373342</t>
+          <t>54426553</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1126,7 +1101,7 @@
         <v>21</v>
       </c>
       <c r="E6" t="n">
-        <v>296</v>
+        <v>340</v>
       </c>
       <c r="F6" t="n">
         <v>99</v>
@@ -1143,11 +1118,11 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>2025</v>
+        <v>2069</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Pavel</t>
+          <t>Павел</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1175,31 +1150,33 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>tomorrow</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="R6" s="2" t="n">
-        <v>45164.41666666666</v>
+        <v>45184.72916666666</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>45164.45833333334</v>
+        <v>45184.77083333334</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PG3W61I7ZYZPRU</t>
+          <t>https://dostavista.ru/track/PG44DZ6LLP25RU</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PGAX4TLP9AIWRU</t>
+          <t>https://dostavista.ru/track/PG3MMDYRR1KWRU</t>
         </is>
       </c>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="n">
-        <v>45363</v>
-      </c>
-      <c r="Y6" t="inlineStr"/>
+        <v>47055</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>47067</v>
+      </c>
       <c r="Z6" t="inlineStr">
         <is>
           <t>canceled</t>
@@ -1207,7 +1184,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>waiting</t>
+          <t>end_with_photo</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
@@ -1215,18 +1192,27 @@
           <t>Смольная</t>
         </is>
       </c>
-      <c r="AC6" t="inlineStr"/>
+      <c r="AC6" t="n">
+        <v>2</v>
+      </c>
       <c r="AD6" t="n">
-        <v>45371</v>
-      </c>
-      <c r="AE6" t="inlineStr"/>
+        <v>47063</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>47071</v>
+      </c>
       <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK32mUETJtes1-mR-BN6RnboeVAePv6AALwzjEbAfkhSEtSV_5bkc17AQADAgADcwADMAQ</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>48fcec99-60d4-46af-be19-21fdf002616a</t>
+          <t>53818456</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1243,7 +1229,7 @@
         <v>21</v>
       </c>
       <c r="E7" t="n">
-        <v>237</v>
+        <v>271</v>
       </c>
       <c r="F7" t="n">
         <v>99</v>
@@ -1260,11 +1246,11 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>1966</v>
+        <v>2000</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Pavel</t>
+          <t>Павел</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1292,39 +1278,41 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>tomorrow</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="R7" s="2" t="n">
-        <v>45164.54166666666</v>
+        <v>45178.41666666666</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>45164.58333333334</v>
+        <v>45178.45833333334</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>будет позже</t>
+          <t>https://dostavista.ru/track/PGD19TYJETLJRU</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>будет позже</t>
+          <t>https://dostavista.ru/track/PGH9SZKICWAJRU</t>
         </is>
       </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="n">
-        <v>45545</v>
-      </c>
-      <c r="Y7" t="inlineStr"/>
+        <v>46408</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>46415</v>
+      </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>будет позже</t>
+          <t>available</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>waiting</t>
+          <t>end_with_photo</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
@@ -1333,15 +1321,22 @@
         </is>
       </c>
       <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="inlineStr"/>
+      <c r="AD7" t="n">
+        <v>46414</v>
+      </c>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK1WmT7jN4AAY3uuHoCrMrSEICyyq2fLAACfdExG-6F4Ut3fmSqkvUvRwEAAwIAA3MAAzAE</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>52401741</t>
+          <t>7fc9866c-4d10-400b-b3f0-edac06b73557</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1358,7 +1353,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="n">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="F8" t="n">
         <v>99</v>
@@ -1375,11 +1370,11 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>1952</v>
+        <v>1993</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Pavel</t>
+          <t>Павел</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1411,32 +1406,30 @@
         </is>
       </c>
       <c r="R8" s="2" t="n">
-        <v>45163.875</v>
+        <v>45182.85416666666</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>45163.91666666666</v>
+        <v>45182.89583333334</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PGA21MWZZTAWRU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>https://dostavista.ru/track/PGEAAI9JKSP5RU</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="n">
-        <v>45678</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>45684</v>
-      </c>
+        <v>46462</v>
+      </c>
+      <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>completed</t>
+          <t>будет позже</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
@@ -1450,27 +1443,16 @@
         </is>
       </c>
       <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="n">
-        <v>45685</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>45686</v>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>252583c3-0872-4709-a532-35feb810c9b9</t>
+          <t>e9ec45ab-af0d-4097-9c54-c37b85e912e0</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1487,7 +1469,7 @@
         <v>21</v>
       </c>
       <c r="E9" t="n">
-        <v>822</v>
+        <v>280</v>
       </c>
       <c r="F9" t="n">
         <v>99</v>
@@ -1504,11 +1486,11 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>2551</v>
+        <v>2009</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Pavel</t>
+          <t>Павел</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1526,12 +1508,12 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>+79859863736</t>
+          <t>+79161052259</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Московская область, Долгопрудный, Первомайская улица, 30к3</t>
+          <t>Москва, Фестивальная улица, 22к7</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1540,10 +1522,10 @@
         </is>
       </c>
       <c r="R9" s="2" t="n">
-        <v>45176.85416666666</v>
+        <v>45182.85416666666</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>45176.89583333334</v>
+        <v>45182.89583333334</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1557,20 +1539,14 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>Я гей</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>Любимому</t>
-        </is>
-      </c>
+          <t>за 10 минут позвонить</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr"/>
       <c r="X9" t="n">
-        <v>45834</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>45840</v>
-      </c>
+        <v>46531</v>
+      </c>
+      <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr">
         <is>
           <t>будет позже</t>
@@ -1591,6 +1567,2755 @@
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>54356137</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>21</v>
+      </c>
+      <c r="E10" t="n">
+        <v>295</v>
+      </c>
+      <c r="F10" t="n">
+        <v>99</v>
+      </c>
+      <c r="G10" t="n">
+        <v>150</v>
+      </c>
+      <c r="H10" t="n">
+        <v>500</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R10" s="2" t="n">
+        <v>45183.875</v>
+      </c>
+      <c r="S10" s="2" t="n">
+        <v>45183.91666666666</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGC1RTFC1AYERU</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PG6E6G9GE1WYRU</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="n">
+        <v>46976</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>46982</v>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>waiting_photo</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="n">
+        <v>46985</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>46986</v>
+      </c>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>aa472169-520f-4f05-959d-4815d8faaf26</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>21</v>
+      </c>
+      <c r="E11" t="n">
+        <v>234</v>
+      </c>
+      <c r="F11" t="n">
+        <v>99</v>
+      </c>
+      <c r="G11" t="n">
+        <v>150</v>
+      </c>
+      <c r="H11" t="n">
+        <v>500</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>1963</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>45183.52083333334</v>
+      </c>
+      <c r="S11" s="2" t="n">
+        <v>45183.5625</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="n">
+        <v>46885</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>46891</v>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>end_collect</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>b19b1e24-dba8-4ffa-9077-00acb648ae3c</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>21</v>
+      </c>
+      <c r="E12" t="n">
+        <v>234</v>
+      </c>
+      <c r="F12" t="n">
+        <v>99</v>
+      </c>
+      <c r="G12" t="n">
+        <v>150</v>
+      </c>
+      <c r="H12" t="n">
+        <v>500</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>1963</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>tomorrow</t>
+        </is>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>45183.41666666666</v>
+      </c>
+      <c r="S12" s="2" t="n">
+        <v>45183.45833333334</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="n">
+        <v>46781</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>46787</v>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>waiting_photo</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>af1e7a63-9a00-4ebc-9eac-79120e6d86de</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>21</v>
+      </c>
+      <c r="E13" t="n">
+        <v>215</v>
+      </c>
+      <c r="F13" t="n">
+        <v>99</v>
+      </c>
+      <c r="G13" t="n">
+        <v>150</v>
+      </c>
+      <c r="H13" t="n">
+        <v>500</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>1944</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>tomorrow</t>
+        </is>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>45184.875</v>
+      </c>
+      <c r="S13" s="2" t="n">
+        <v>45184.91666666666</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="n">
+        <v>46949</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>46955</v>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>end_collect</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>e064a6e0-d416-4d2a-902d-8b4de9d71483</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>21</v>
+      </c>
+      <c r="E14" t="n">
+        <v>215</v>
+      </c>
+      <c r="F14" t="n">
+        <v>99</v>
+      </c>
+      <c r="G14" t="n">
+        <v>150</v>
+      </c>
+      <c r="H14" t="n">
+        <v>500</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>1944</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>tomorrow</t>
+        </is>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>45184.625</v>
+      </c>
+      <c r="S14" s="2" t="n">
+        <v>45184.66666666666</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="n">
+        <v>46915</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>46921</v>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>будет позже</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>end_collect</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>54357550</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="n">
+        <v>295</v>
+      </c>
+      <c r="F15" t="n">
+        <v>99</v>
+      </c>
+      <c r="G15" t="n">
+        <v>150</v>
+      </c>
+      <c r="H15" t="n">
+        <v>500</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>45183.875</v>
+      </c>
+      <c r="S15" s="2" t="n">
+        <v>45183.91666666666</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGG3LG333HNZRU</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGAS3MFS3MD5RU</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="n">
+        <v>47014</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>47031</v>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>canceled</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>end_with_photo</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="n">
+        <v>47022</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>47035</v>
+      </c>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK3tmUDMkEhI-BTHG93undpB-J2Q-Y4AAIwzzEbAfkZSELMdI3Je9FPAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>54434008</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>21</v>
+      </c>
+      <c r="E16" t="n">
+        <v>209</v>
+      </c>
+      <c r="F16" t="n">
+        <v>99</v>
+      </c>
+      <c r="G16" t="n">
+        <v>150</v>
+      </c>
+      <c r="H16" t="n">
+        <v>500</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>1938</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>tomorrow</t>
+        </is>
+      </c>
+      <c r="R16" s="2" t="n">
+        <v>45185.875</v>
+      </c>
+      <c r="S16" s="2" t="n">
+        <v>45185.91666666666</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGC3GJTDTTMDRU</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGGLGP4LW1NKRU</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="n">
+        <v>47092</v>
+      </c>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>canceled</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>47097</v>
+      </c>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>954178da04834db38d0f36ba84310299</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>21</v>
+      </c>
+      <c r="E17" t="n">
+        <v>826</v>
+      </c>
+      <c r="F17" t="n">
+        <v>99</v>
+      </c>
+      <c r="G17" t="n">
+        <v>150</v>
+      </c>
+      <c r="H17" t="n">
+        <v>500</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>2555</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>45184.69722222222</v>
+      </c>
+      <c r="S17" s="2" t="n">
+        <v>45184.73888888889</v>
+      </c>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="n">
+        <v>47204</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>47210</v>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>a5845dbaa54042e6b848308d727f0794</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>21</v>
+      </c>
+      <c r="E18" t="n">
+        <v>686</v>
+      </c>
+      <c r="F18" t="n">
+        <v>99</v>
+      </c>
+      <c r="G18" t="n">
+        <v>150</v>
+      </c>
+      <c r="H18" t="n">
+        <v>500</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>2415</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R18" s="2" t="n">
+        <v>45184.71041666667</v>
+      </c>
+      <c r="S18" s="2" t="n">
+        <v>45184.75208333333</v>
+      </c>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="n">
+        <v>47228</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>47234</v>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>waiting_photo</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>4ba51b0151e349fcb3fd96859d97297e</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>21</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1690</v>
+      </c>
+      <c r="F19" t="n">
+        <v>99</v>
+      </c>
+      <c r="G19" t="n">
+        <v>150</v>
+      </c>
+      <c r="H19" t="n">
+        <v>500</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>3419</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>45207.88194444445</v>
+      </c>
+      <c r="S19" s="2" t="n">
+        <v>45207.92361111111</v>
+      </c>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="n">
+        <v>47683</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>47687</v>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>54873281</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>21</v>
+      </c>
+      <c r="E20" t="n">
+        <v>335</v>
+      </c>
+      <c r="F20" t="n">
+        <v>99</v>
+      </c>
+      <c r="G20" t="n">
+        <v>150</v>
+      </c>
+      <c r="H20" t="n">
+        <v>500</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>2064</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R20" s="2" t="n">
+        <v>45189.72916666666</v>
+      </c>
+      <c r="S20" s="2" t="n">
+        <v>45189.77083333334</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PG7GC5EWTWYERU</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGI7C73PJYT4RU</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="n">
+        <v>47266</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>47272</v>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>canceled</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="n">
+        <v>47274</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>47275</v>
+      </c>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>56655315</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>21</v>
+      </c>
+      <c r="E21" t="n">
+        <v>363</v>
+      </c>
+      <c r="F21" t="n">
+        <v>99</v>
+      </c>
+      <c r="G21" t="n">
+        <v>150</v>
+      </c>
+      <c r="H21" t="n">
+        <v>500</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>2092</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R21" s="2" t="n">
+        <v>45207.72916666666</v>
+      </c>
+      <c r="S21" s="2" t="n">
+        <v>45207.77083333334</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PG4EFDKWZKCSRU</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PG5EYW76N9LWRU</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="n">
+        <v>47456</v>
+      </c>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>canceled</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="n">
+        <v>47462</v>
+      </c>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>56657969</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>21</v>
+      </c>
+      <c r="E22" t="n">
+        <v>363</v>
+      </c>
+      <c r="F22" t="n">
+        <v>99</v>
+      </c>
+      <c r="G22" t="n">
+        <v>150</v>
+      </c>
+      <c r="H22" t="n">
+        <v>500</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>2092</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R22" s="2" t="n">
+        <v>45207.72916666666</v>
+      </c>
+      <c r="S22" s="2" t="n">
+        <v>45207.77083333334</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGH6IRLI3FEJRU</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PG3Y9HTWCFD6RU</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>За 10 минут до доставки, позвонить</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="n">
+        <v>47557</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>47571</v>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>end_with_photo</t>
+        </is>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>47563</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>47573</v>
+      </c>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AH22" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK50mUip5QMpF6xKMNJ-kEJDCKi1JfxAAJtzDEbi7QQScY1a8q9cMkyAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0149d6d5cc94478cb94672ad9e5646bb</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" t="n">
+        <v>730</v>
+      </c>
+      <c r="F23" t="n">
+        <v>99</v>
+      </c>
+      <c r="G23" t="n">
+        <v>150</v>
+      </c>
+      <c r="H23" t="n">
+        <v>500</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>2459</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R23" s="2" t="n">
+        <v>45207.64027777778</v>
+      </c>
+      <c r="S23" s="2" t="n">
+        <v>45207.68194444444</v>
+      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="n">
+        <v>47482</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>47488</v>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>waiting_photo</t>
+        </is>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>39bea7d38f4542beb22d92971133fc93</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>21</v>
+      </c>
+      <c r="E24" t="n">
+        <v>714</v>
+      </c>
+      <c r="F24" t="n">
+        <v>99</v>
+      </c>
+      <c r="G24" t="n">
+        <v>150</v>
+      </c>
+      <c r="H24" t="n">
+        <v>500</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>2443</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Александр</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>+79119648410</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 13к1</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R24" s="2" t="n">
+        <v>45210.54305555556</v>
+      </c>
+      <c r="S24" s="2" t="n">
+        <v>45210.58472222222</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>https://mipt.ru/education/chair/military/about/</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>https://mipt.ru/education/chair/military/about/</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>за 10 минут до доставки позвонить</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="n">
+        <v>47905</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>47921</v>
+      </c>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>end_with_photo</t>
+        </is>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="n">
+        <v>47929</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>47924</v>
+      </c>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>78903042259</t>
+        </is>
+      </c>
+      <c r="AH24" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK7MGUmcu60nttuUR0lxbxcMi-ZsEZKAAKx0TEbCiw5SRyHsVRS0juWAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>54874141</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>21</v>
+      </c>
+      <c r="E25" t="n">
+        <v>335</v>
+      </c>
+      <c r="F25" t="n">
+        <v>99</v>
+      </c>
+      <c r="G25" t="n">
+        <v>150</v>
+      </c>
+      <c r="H25" t="n">
+        <v>500</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>2064</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Pavel</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>45189.72916666666</v>
+      </c>
+      <c r="S25" s="2" t="n">
+        <v>45189.77083333334</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGCCGCIGANNJRU</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGCS5XHCX5M4RU</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>ничего не надо</t>
+        </is>
+      </c>
+      <c r="X25" t="n">
+        <v>47336</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>47348</v>
+      </c>
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>canceled</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>end_with_photo</t>
+        </is>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC25" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>47344</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>47352</v>
+      </c>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK482UK6NbsOax7ZZDCqedVGWnqXRQNAAJhzzEb7GpYSJctDBogBZTJAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>56700728</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>21</v>
+      </c>
+      <c r="E26" t="n">
+        <v>436</v>
+      </c>
+      <c r="F26" t="n">
+        <v>99</v>
+      </c>
+      <c r="G26" t="n">
+        <v>150</v>
+      </c>
+      <c r="H26" t="n">
+        <v>500</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>2165</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Today</t>
+        </is>
+      </c>
+      <c r="R26" s="2" t="n">
+        <v>45207.875</v>
+      </c>
+      <c r="S26" s="2" t="n">
+        <v>45207.91666666666</v>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGM1HYW1IT7SRU</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>https://dostavista.ru/track/PGCRD3A2D57GRU</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="n">
+        <v>47592</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>47603</v>
+      </c>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>canceled</t>
+        </is>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>end_with_photo</t>
+        </is>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC26" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>47598</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>47605</v>
+      </c>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK58mUi1BOwKC7kOMkQFAPJUb5Tfo7fAAJtzDEbi7QQScY1a8q9cMkyAQADAgADcwADMAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>d3e883bc502243369b002598f4cfe772</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>21</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1524</v>
+      </c>
+      <c r="F27" t="n">
+        <v>99</v>
+      </c>
+      <c r="G27" t="n">
+        <v>150</v>
+      </c>
+      <c r="H27" t="n">
+        <v>500</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>3253</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>45207.82986111111</v>
+      </c>
+      <c r="S27" s="2" t="n">
+        <v>45207.87152777778</v>
+      </c>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="n">
+        <v>47623</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>47627</v>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0e1648215c114a1b897059c4d7758057</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>21</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1882</v>
+      </c>
+      <c r="F28" t="n">
+        <v>99</v>
+      </c>
+      <c r="G28" t="n">
+        <v>150</v>
+      </c>
+      <c r="H28" t="n">
+        <v>500</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>3611</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R28" s="2" t="n">
+        <v>45208.02777777778</v>
+      </c>
+      <c r="S28" s="2" t="n">
+        <v>45208.06944444445</v>
+      </c>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="n">
+        <v>47707</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>47712</v>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>waiting_photo</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>36f7c8fe8d8c4ea0b5aca2c3ba3f03d0</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>21</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1459</v>
+      </c>
+      <c r="F29" t="n">
+        <v>99</v>
+      </c>
+      <c r="G29" t="n">
+        <v>150</v>
+      </c>
+      <c r="H29" t="n">
+        <v>500</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>3188</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Павел</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 22к7</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R29" s="2" t="n">
+        <v>45207.86180555556</v>
+      </c>
+      <c r="S29" s="2" t="n">
+        <v>45207.90347222222</v>
+      </c>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="n">
+        <v>47661</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>47665</v>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>e63d196384b3450ea1a818fc1ca8a3b3</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>21</v>
+      </c>
+      <c r="E30" t="n">
+        <v>383</v>
+      </c>
+      <c r="F30" t="n">
+        <v>99</v>
+      </c>
+      <c r="G30" t="n">
+        <v>150</v>
+      </c>
+      <c r="H30" t="n">
+        <v>500</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>2112</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Александр</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>+79119648410</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 13к1</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>45210.74652777778</v>
+      </c>
+      <c r="S30" s="2" t="n">
+        <v>45210.78819444445</v>
+      </c>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>за 10 минут до доставки позвонить</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="n">
+        <v>47946</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>47951</v>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>waiting</t>
+        </is>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>c2814c32c4164924872b564ce9fb2006</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>21</v>
+      </c>
+      <c r="E31" t="n">
+        <v>624</v>
+      </c>
+      <c r="F31" t="n">
+        <v>99</v>
+      </c>
+      <c r="G31" t="n">
+        <v>150</v>
+      </c>
+      <c r="H31" t="n">
+        <v>500</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>2353</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Александр</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>+79119648410</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 13к1</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R31" s="2" t="n">
+        <v>45210.52361111111</v>
+      </c>
+      <c r="S31" s="2" t="n">
+        <v>45210.56527777778</v>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>https://mipt.ru/education/chair/military/about/</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>https://mipt.ru/education/chair/military/about/</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>за 10 минут до доставки позвонить</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="n">
+        <v>47833</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>47838</v>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>waiting_photo</t>
+        </is>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="n">
+        <v>47847</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>47848</v>
+      </c>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t>79161052259</t>
+        </is>
+      </c>
+      <c r="AH31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>c61fe3f6718f422cbd7f0c35a969a805</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>rose_silva_pink</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Розы Silva Pink</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>21</v>
+      </c>
+      <c r="E32" t="n">
+        <v>472</v>
+      </c>
+      <c r="F32" t="n">
+        <v>99</v>
+      </c>
+      <c r="G32" t="n">
+        <v>150</v>
+      </c>
+      <c r="H32" t="n">
+        <v>500</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>2201</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Александр</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>+79161052259</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>paveldibr</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>310251240</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>+79119648410</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Москва, Фестивальная улица, 13к1</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>Express</t>
+        </is>
+      </c>
+      <c r="R32" s="2" t="n">
+        <v>45210.74930555555</v>
+      </c>
+      <c r="S32" s="2" t="n">
+        <v>45210.79097222222</v>
+      </c>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>за 10 минут до доставки позвонить</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="n">
+        <v>47985</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>48001</v>
+      </c>
+      <c r="Z32" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>end_with_photo</t>
+        </is>
+      </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>Смольная</t>
+        </is>
+      </c>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="n">
+        <v>48005</v>
+      </c>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t>AgACAgIAAxkBAAK7fmUmvbxx_RdYSKx6pGjyxwsaZE5aAALB0zEbCiw5SUmN1kEfoIEuAQADAgADcwADMAQ</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>